<commit_message>
Registro de un usuario completo
</commit_message>
<xml_diff>
--- a/Resources/datapool/TitulosPaginas.xlsx
+++ b/Resources/datapool/TitulosPaginas.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Titulo</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Cruises</t>
+  </si>
+  <si>
+    <t>Register: Mercury Tours</t>
+  </si>
+  <si>
+    <t>Registro</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,6 +168,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -181,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -250,6 +260,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>